<commit_message>
Updated Balance Sheet df
</commit_message>
<xml_diff>
--- a/src/(EXCEL) MSFT: income_statement_data.xlsx
+++ b/src/(EXCEL) MSFT: income_statement_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="income_statement_data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MSFT income_statement_data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,724 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>{</t>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2023-06-30_FY</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2022-06-30_FY</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2021-06-30_FY</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2020-06-30_FY</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2019-06-30_FY</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  "Error Message": "Limit Reach . Please upgrade your plan or visit our documentation for more details at https://site.financialmodelingprep.com/"</t>
-        </is>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>211915000000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>198270000000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>168088000000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>143015000000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>125843000000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>}</t>
-        </is>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>costOfRevenue</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>65863000000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>62650000000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>52232000000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>46078000000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>42910000000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>grossProfit</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>146052000000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>135620000000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>115856000000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>96937000000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>82933000000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>grossProfitRatio</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.6892008588</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.6840167448</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6892580077</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6778100199</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6590195720000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>COST And EXPENSES</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ResearchAndDevelopmentExpenses</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>27195000000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>24512000000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20716000000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>19269000000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>16876000000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GeneralAndAdministrativeExpenses</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>7575000000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5900000000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5107000000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5111000000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4885000000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SellingAndMarketingExpenses</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>22759000000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>21825000000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20117000000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>19598000000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>18213000000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>otherExpenses</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>788000000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>333000000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1186000000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>77000000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>operatingExpenses</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>57740000000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>51951000000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>44555000000</v>
+      </c>
+      <c r="F12" t="n">
+        <v>43990000000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>39321000000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>costAndExpenses</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>123603000000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>114601000000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>96787000000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>90068000000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>82231000000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>interestExpense</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1968000000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2063000000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2346000000</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2591000000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2686000000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>depreciationAndAmortization</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>13500000000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>14600000000</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10900000000</v>
+      </c>
+      <c r="F17" t="n">
+        <v>12300000000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>11600000000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>102023000000</v>
+      </c>
+      <c r="D18" t="n">
+        <v>97983000000</v>
+      </c>
+      <c r="E18" t="n">
+        <v>80816000000</v>
+      </c>
+      <c r="F18" t="n">
+        <v>65259000000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>54559000000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>EBITDARatio</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.4814335937</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.4941897413</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4807957736</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.4563087788</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.4335481513</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>INCOME</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>operatingIncome</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>88523000000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>83383000000</v>
+      </c>
+      <c r="E22" t="n">
+        <v>69916000000</v>
+      </c>
+      <c r="F22" t="n">
+        <v>52959000000</v>
+      </c>
+      <c r="G22" t="n">
+        <v>42959000000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>operatingIncomeRatio</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4177288064</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.4205527816</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.4159487887</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3703038143</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.3413698021</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>totalOtherIncomeExpensesNet</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>788000000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>333000000</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1186000000</v>
+      </c>
+      <c r="F24" t="n">
+        <v>77000000</v>
+      </c>
+      <c r="G24" t="n">
+        <v>729000000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>incomeBeforeTax</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>89311000000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>83716000000</v>
+      </c>
+      <c r="E25" t="n">
+        <v>71102000000</v>
+      </c>
+      <c r="F25" t="n">
+        <v>53036000000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>43688000000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>incomeBeforeTaxRatio</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.4214472784</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.4222323095</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.4230046166</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3708422193</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.3471627345</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>incomeTaxExpense</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>16950000000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10978000000</v>
+      </c>
+      <c r="E27" t="n">
+        <v>9831000000</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8755000000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4448000000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>netIncome</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>72361000000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>72738000000</v>
+      </c>
+      <c r="E28" t="n">
+        <v>61271000000</v>
+      </c>
+      <c r="F28" t="n">
+        <v>44281000000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>39240000000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>netIncomeRatio</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.3414623788</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.3668633681</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.3645173956</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.3096248645</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.3118171054</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>EPS</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>EPS</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="D32" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="E32" t="n">
+        <v>8.119999999999999</v>
+      </c>
+      <c r="F32" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5.06</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>EPSDiluted</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>9.68</v>
+      </c>
+      <c r="D33" t="n">
+        <v>9.65</v>
+      </c>
+      <c r="E33" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5.06</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>weightedAverageShsOut</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>7475309917</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7537616580</v>
+      </c>
+      <c r="E34" t="n">
+        <v>7611304347</v>
+      </c>
+      <c r="F34" t="n">
+        <v>7687673611</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7754940711</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>weightedAverageShsOutDil</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>7472000000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>7540000000</v>
+      </c>
+      <c r="E35" t="n">
+        <v>7608000000</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7683000000</v>
+      </c>
+      <c r="G35" t="n">
+        <v>7753000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>